<commit_message>
played with parameters a and b, and decided to explore each separately, with other being zero. Added dummy_convergence_plot code to demonstrate how parameters a and b can degrade (logaritmically) over time (per round).
</commit_message>
<xml_diff>
--- a/measurements/results/result_spreadsheet.xlsx
+++ b/measurements/results/result_spreadsheet.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DH2"/>
+  <dimension ref="A1:DH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1524,6 +1524,1082 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.5805749790748964</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.7942942102568505</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.6116847468948932</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.1458389249337071</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.3532209859925364</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 47.7760 , 4.9053 , 60</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 97.8104 , 5.1732 , 123</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 112.8947 , 5.5357 , 142</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 96.2194 , 5.2857 , 121</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>100 , 120.8628 , 4.4643 , 152</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 50.9471 , 5.1732 , 64</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="Y3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="Z3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 93.0531 , 4.8095 , 117</t>
+        </is>
+      </c>
+      <c r="AA3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="AB3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AC3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="AD3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AE3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 96.2194 , 5.2857 , 121</t>
+        </is>
+      </c>
+      <c r="AF3" s="1" t="inlineStr">
+        <is>
+          <t>200 , 112.9198 , 4.4643 , 142</t>
+        </is>
+      </c>
+      <c r="AG3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 47.7760 , 4.9053 , 60</t>
+        </is>
+      </c>
+      <c r="AH3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="AI3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="AJ3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 93.0531 , 4.8095 , 117</t>
+        </is>
+      </c>
+      <c r="AK3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="AL3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AM3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="AN3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AO3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 99.3966 , 5.2857 , 125</t>
+        </is>
+      </c>
+      <c r="AP3" s="1" t="inlineStr">
+        <is>
+          <t>300 , 120.8628 , 4.4643 , 152</t>
+        </is>
+      </c>
+      <c r="AQ3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 37.4397 , 5.3815 , 47</t>
+        </is>
+      </c>
+      <c r="AR3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="AS3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="AT3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 97.8104 , 5.1732 , 123</t>
+        </is>
+      </c>
+      <c r="AU3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="AV3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AW3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="AX3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="AY3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 92.2480 , 5.2857 , 116</t>
+        </is>
+      </c>
+      <c r="AZ3" s="1" t="inlineStr">
+        <is>
+          <t>400 , 123.2457 , 4.4643 , 155</t>
+        </is>
+      </c>
+      <c r="BA3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 50.9471 , 5.1732 , 64</t>
+        </is>
+      </c>
+      <c r="BB3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="BC3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="BD3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 93.0531 , 4.8095 , 117</t>
+        </is>
+      </c>
+      <c r="BE3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="BF3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="BG3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="BH3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="BI3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 92.2480 , 5.2857 , 116</t>
+        </is>
+      </c>
+      <c r="BJ3" s="1" t="inlineStr">
+        <is>
+          <t>500 , 120.8578 , 4.6429 , 152</t>
+        </is>
+      </c>
+      <c r="BK3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 50.9471 , 5.1732 , 64</t>
+        </is>
+      </c>
+      <c r="BL3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="BM3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="BN3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 93.0531 , 4.8095 , 117</t>
+        </is>
+      </c>
+      <c r="BO3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="BP3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="BQ3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="BR3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="BS3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 96.2194 , 5.2857 , 121</t>
+        </is>
+      </c>
+      <c r="BT3" s="1" t="inlineStr">
+        <is>
+          <t>600 , 123.2457 , 4.4643 , 155</t>
+        </is>
+      </c>
+      <c r="BU3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 52.5313 , 5.3815 , 66</t>
+        </is>
+      </c>
+      <c r="BV3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="BW3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="BX3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 97.8104 , 5.1732 , 123</t>
+        </is>
+      </c>
+      <c r="BY3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="BZ3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CA3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="CB3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CC3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 92.2480 , 5.2857 , 116</t>
+        </is>
+      </c>
+      <c r="CD3" s="1" t="inlineStr">
+        <is>
+          <t>700 , 123.2457 , 4.4643 , 155</t>
+        </is>
+      </c>
+      <c r="CE3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 45.3640 , 6.5065 , 57</t>
+        </is>
+      </c>
+      <c r="CF3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="CG3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="CH3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 93.0514 , 4.8810 , 117</t>
+        </is>
+      </c>
+      <c r="CI3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="CJ3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CK3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="CL3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CM3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 103.3681 , 5.2857 , 130</t>
+        </is>
+      </c>
+      <c r="CN3" s="1" t="inlineStr">
+        <is>
+          <t>800 , 112.9198 , 4.4643 , 142</t>
+        </is>
+      </c>
+      <c r="CO3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 50.9471 , 5.1732 , 64</t>
+        </is>
+      </c>
+      <c r="CP3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="CQ3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="CR3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 94.6417 , 4.8095 , 119</t>
+        </is>
+      </c>
+      <c r="CS3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="CT3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CU3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="CV3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="CW3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 92.2480 , 5.2857 , 116</t>
+        </is>
+      </c>
+      <c r="CX3" s="1" t="inlineStr">
+        <is>
+          <t>900 , 123.2457 , 4.4643 , 155</t>
+        </is>
+      </c>
+      <c r="CY3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 50.9471 , 5.1732 , 64</t>
+        </is>
+      </c>
+      <c r="CZ3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="DA3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 102.5797 , 5.0179 , 129</t>
+        </is>
+      </c>
+      <c r="DB3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 97.8104 , 5.1732 , 123</t>
+        </is>
+      </c>
+      <c r="DC3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 122.4535 , 4.3929 , 154</t>
+        </is>
+      </c>
+      <c r="DD3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="DE3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 130.3691 , 5.5357 , 164</t>
+        </is>
+      </c>
+      <c r="DF3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 142.2835 , 5.5357 , 179</t>
+        </is>
+      </c>
+      <c r="DG3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 96.2194 , 5.2857 , 121</t>
+        </is>
+      </c>
+      <c r="DH3" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 120.8628 , 4.4643 , 152</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.1284803202380342</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.04010278080410157</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.8432405951299429</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.5267426977749526</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.7480310273503831</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 5.994 , 6.875 , 149</t>
+        </is>
+      </c>
+      <c r="N4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="O4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="P4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="Q4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="R4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.196 , 6.518 , 154</t>
+        </is>
+      </c>
+      <c r="S4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.804 , 4.904 , 169</t>
+        </is>
+      </c>
+      <c r="T4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="U4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 6.128 , 3.946 , 152</t>
+        </is>
+      </c>
+      <c r="V4" s="1" t="inlineStr">
+        <is>
+          <t>100 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="W4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.398 , 6.029 , 159</t>
+        </is>
+      </c>
+      <c r="X4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="Y4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.157 , 6.042 , 153</t>
+        </is>
+      </c>
+      <c r="Z4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="AA4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="AB4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.196 , 6.518 , 154</t>
+        </is>
+      </c>
+      <c r="AC4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="AD4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="AE4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 6.362 , 4.904 , 158</t>
+        </is>
+      </c>
+      <c r="AF4" s="1" t="inlineStr">
+        <is>
+          <t>200 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="AG4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.394 , 7.375 , 159</t>
+        </is>
+      </c>
+      <c r="AH4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="AI4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="AJ4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="AK4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="AL4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.196 , 6.518 , 154</t>
+        </is>
+      </c>
+      <c r="AM4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="AN4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="AO4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 6.721 , 5.417 , 167</t>
+        </is>
+      </c>
+      <c r="AP4" s="1" t="inlineStr">
+        <is>
+          <t>300 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="AQ4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.398 , 6.029 , 159</t>
+        </is>
+      </c>
+      <c r="AR4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="AS4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.317 , 6.250 , 157</t>
+        </is>
+      </c>
+      <c r="AT4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="AU4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="AV4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 5.393 , 6.518 , 134</t>
+        </is>
+      </c>
+      <c r="AW4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="AX4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="AY4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 6.718 , 6.042 , 167</t>
+        </is>
+      </c>
+      <c r="AZ4" s="1" t="inlineStr">
+        <is>
+          <t>400 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="BA4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.474 , 7.375 , 161</t>
+        </is>
+      </c>
+      <c r="BB4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="BC4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="BD4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="BE4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="BF4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 5.193 , 6.518 , 129</t>
+        </is>
+      </c>
+      <c r="BG4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="BH4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="BI4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 6.560 , 5.530 , 163</t>
+        </is>
+      </c>
+      <c r="BJ4" s="1" t="inlineStr">
+        <is>
+          <t>500 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="BK4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.079 , 5.529 , 151</t>
+        </is>
+      </c>
+      <c r="BL4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="BM4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="BN4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="BO4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="BP4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 5.394 , 6.310 , 134</t>
+        </is>
+      </c>
+      <c r="BQ4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="BR4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.725 , 4.696 , 167</t>
+        </is>
+      </c>
+      <c r="BS4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 6.562 , 5.017 , 163</t>
+        </is>
+      </c>
+      <c r="BT4" s="1" t="inlineStr">
+        <is>
+          <t>600 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="BU4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.801 , 5.529 , 169</t>
+        </is>
+      </c>
+      <c r="BV4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="BW4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="BX4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="BY4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="BZ4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 5.475 , 6.006 , 136</t>
+        </is>
+      </c>
+      <c r="CA4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="CB4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="CC4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 6.364 , 4.696 , 158</t>
+        </is>
+      </c>
+      <c r="CD4" s="1" t="inlineStr">
+        <is>
+          <t>700 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="CE4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.074 , 6.875 , 151</t>
+        </is>
+      </c>
+      <c r="CF4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="CG4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 5.956 , 6.250 , 148</t>
+        </is>
+      </c>
+      <c r="CH4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="CI4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="CJ4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.196 , 6.518 , 154</t>
+        </is>
+      </c>
+      <c r="CK4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="CL4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.804 , 4.904 , 169</t>
+        </is>
+      </c>
+      <c r="CM4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 6.925 , 4.696 , 172</t>
+        </is>
+      </c>
+      <c r="CN4" s="1" t="inlineStr">
+        <is>
+          <t>800 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="CO4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.398 , 6.029 , 159</t>
+        </is>
+      </c>
+      <c r="CP4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="CQ4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="CR4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="CS4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.961 , 5.529 , 173</t>
+        </is>
+      </c>
+      <c r="CT4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 5.193 , 6.518 , 129</t>
+        </is>
+      </c>
+      <c r="CU4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="CV4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="CW4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 6.720 , 5.529 , 167</t>
+        </is>
+      </c>
+      <c r="CX4" s="1" t="inlineStr">
+        <is>
+          <t>900 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+      <c r="CY4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.478 , 6.029 , 161</t>
+        </is>
+      </c>
+      <c r="CZ4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="DA4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.958 , 6.250 , 173</t>
+        </is>
+      </c>
+      <c r="DB4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.602 , 5.172 , 164</t>
+        </is>
+      </c>
+      <c r="DC4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.523 , 4.904 , 162</t>
+        </is>
+      </c>
+      <c r="DD4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 5.393 , 6.518 , 134</t>
+        </is>
+      </c>
+      <c r="DE4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="DF4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 6.723 , 4.904 , 167</t>
+        </is>
+      </c>
+      <c r="DG4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 5.518 , 5.321 , 137</t>
+        </is>
+      </c>
+      <c r="DH4" s="1" t="inlineStr">
+        <is>
+          <t>1000 , 7.601 , 6.029 , 189</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>